<commit_message>
Quan-update SRS các phần
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Project</t>
   </si>
@@ -384,6 +384,18 @@
   </si>
   <si>
     <t>1 phần SRS</t>
+  </si>
+  <si>
+    <t>21/9/2012</t>
+  </si>
+  <si>
+    <t>Tổng hợp các phần của SRS thành báo cáo nhóm, gửi bài nộp lên sakai</t>
+  </si>
+  <si>
+    <t>SRS version 1.0</t>
+  </si>
+  <si>
+    <t>Xong</t>
   </si>
 </sst>
 </file>
@@ -3100,7 +3112,7 @@
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4272,11 +4284,15 @@
       <c r="C5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="E5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9">
+        <v>4</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -5296,10 +5312,16 @@
       <c r="AMI5" s="11"/>
       <c r="AMJ5" s="11"/>
     </row>
-    <row r="6" spans="1:1024" s="12" customFormat="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+    <row r="6" spans="1:1024" s="12" customFormat="1" ht="28.5">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>

</xml_diff>

<commit_message>
refactor contact page, about pages. search page
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>Project</t>
   </si>
@@ -428,10 +428,22 @@
     <t>Hiện thực module search</t>
   </si>
   <si>
-    <t>29/10/2012</t>
+    <t>module search</t>
   </si>
   <si>
-    <t>module search</t>
+    <t>27/11/2012</t>
+  </si>
+  <si>
+    <t>chưa test</t>
+  </si>
+  <si>
+    <t>28/11/2012</t>
+  </si>
+  <si>
+    <t>Page About</t>
+  </si>
+  <si>
+    <t>Page Contact</t>
   </si>
 </sst>
 </file>
@@ -3151,7 +3163,7 @@
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10541,19 +10553,23 @@
     </row>
     <row r="11" spans="1:1024" s="12" customFormat="1">
       <c r="A11" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E11" s="9">
         <v>8</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>3</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -11574,12 +11590,24 @@
       <c r="AMJ11" s="11"/>
     </row>
     <row r="12" spans="1:1024" s="12" customFormat="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>2</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -12600,12 +12628,24 @@
       <c r="AMJ12" s="11"/>
     </row>
     <row r="13" spans="1:1024" s="12" customFormat="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>2</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>

</xml_diff>

<commit_message>
huỷ mượn sách thêm trường vào user info
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>Project</t>
   </si>
@@ -459,6 +459,21 @@
   </si>
   <si>
     <t>final report</t>
+  </si>
+  <si>
+    <t>30/11/2012</t>
+  </si>
+  <si>
+    <t>implement mượn sách</t>
+  </si>
+  <si>
+    <t>module mượn sách</t>
+  </si>
+  <si>
+    <t>implement huỷ mượn sách</t>
+  </si>
+  <si>
+    <t>module huỷ mượn</t>
   </si>
 </sst>
 </file>
@@ -3177,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16793,12 +16808,24 @@
       <c r="AMJ16" s="11"/>
     </row>
     <row r="17" spans="1:1024" s="12" customFormat="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4</v>
+      </c>
+      <c r="F17" s="9">
+        <v>4</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -17819,12 +17846,24 @@
       <c r="AMJ17" s="11"/>
     </row>
     <row r="18" spans="1:1024" s="12" customFormat="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="9">
+        <v>2</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>

</xml_diff>

<commit_message>
layout for admin page will make layout for book page soon
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
   <si>
     <t>Project</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>module history user</t>
+  </si>
+  <si>
+    <t>layout for admin page</t>
+  </si>
+  <si>
+    <t>layout admin</t>
   </si>
 </sst>
 </file>
@@ -3198,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -19928,12 +19934,24 @@
       <c r="AMJ19" s="11"/>
     </row>
     <row r="20" spans="1:1024" s="12" customFormat="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="9">
+        <v>2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>3</v>
+      </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>

</xml_diff>

<commit_message>
sửa layout, thêm button,
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>Project</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>layout admin</t>
+  </si>
+  <si>
+    <t>implement nhận sách/trả sách</t>
+  </si>
+  <si>
+    <t>receive/return book</t>
   </si>
 </sst>
 </file>
@@ -3205,7 +3211,7 @@
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -20972,12 +20978,24 @@
       <c r="AMJ20" s="11"/>
     </row>
     <row r="21" spans="1:1024" s="12" customFormat="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="A21" s="14">
+        <v>40980</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="9">
+        <v>3</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>

</xml_diff>

<commit_message>
sửa phân quyền nick admin:admin@crazylib.com pass 123456 hoặc nhoxti125@gmail.com pass 123456
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Quan.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
   <si>
     <t>Project</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>receive/return book</t>
+  </si>
+  <si>
+    <t>implement phân quyền</t>
+  </si>
+  <si>
+    <t>phân quyền</t>
   </si>
 </sst>
 </file>
@@ -3210,8 +3216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3248,7 +3254,9 @@
         <v>33</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="15"/>
+      <c r="F1" s="15">
+        <v>50902143</v>
+      </c>
       <c r="G1" s="15"/>
       <c r="P1" s="4" t="s">
         <v>3</v>
@@ -22016,12 +22024,24 @@
       <c r="AMJ21" s="11"/>
     </row>
     <row r="22" spans="1:1024" s="12" customFormat="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="14">
+        <v>41011</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="9">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9">
+        <v>4</v>
+      </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>

</xml_diff>